<commit_message>
Eagle lib update & logos
</commit_message>
<xml_diff>
--- a/misc/CopterSizing.xlsx
+++ b/misc/CopterSizing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="6680" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2000" yWindow="2260" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Châssis</t>
   </si>
@@ -147,13 +147,34 @@
   </si>
   <si>
     <t>Prop</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Hélices</t>
+  </si>
+  <si>
+    <t>Diamètre</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Pas</t>
+  </si>
+  <si>
+    <t>Nb. Pales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00\ _g"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,21 +206,300 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -232,17 +532,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -640,10 +969,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -653,259 +982,298 @@
     <col min="6" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="1" spans="1:7" ht="16" thickBot="1"/>
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1">
+      <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="C3" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="28">
         <v>297</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="10">
         <v>4</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="22">
         <f>kp_bat*bat_charge_tot*bat_s*bat_p</f>
         <v>396</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F9">
+      <c r="E9" s="7"/>
+      <c r="F9" s="14">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="22">
         <f>mot_poids*uav_n_rotor</f>
         <v>280</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="14">
         <v>3300</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
-        <f>esc_courant_max*kp_esc</f>
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="22">
+        <f>esc_courant_max*kp_esc*uav_n_rotor</f>
+        <v>156</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="E11" s="7"/>
+      <c r="F11" s="14">
         <v>3.7</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" ht="16" thickBot="1">
+      <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="24">
         <f>poids_accu+poids_moteur+poids_esc</f>
-        <v>715</v>
-      </c>
-      <c r="C12" t="s">
+        <v>832</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="22">
         <f>bat_capacite_el*bat_p</f>
         <v>3300</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="F13">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
+      <c r="A13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="27">
+        <f>poids_prop+poids_chassis</f>
+        <v>1129</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="22">
         <f>bat_tension_el*bat_s</f>
         <v>14.8</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="E14" t="s">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
+      <c r="E14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="14">
         <v>65</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="E15" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="E15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="16">
         <v>100</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="18">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7" ht="16" thickBot="1">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="20">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="16" thickBot="1">
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16" thickBot="1">
+      <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="10">
         <v>840</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="14">
         <v>0.4</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="14">
         <v>10</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="14">
         <v>18</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
+      <c r="A24" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="16">
         <v>70</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="17" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E17:G17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>